<commit_message>
Just taking care of some activities
</commit_message>
<xml_diff>
--- a/Semestre 1/2.- Probabilidad Y Estadística/ejercicios nueve febrero.xlsx
+++ b/Semestre 1/2.- Probabilidad Y Estadística/ejercicios nueve febrero.xlsx
@@ -1,14 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Villaseñor\Documents\TecTepic\Semestre 1\2.- Probabilidad Y Estadística\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E46AA89-D5DB-4CDD-A6B8-673C320E24F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -27,35 +34,35 @@
     <t>-0.9103694</t>
   </si>
   <si>
-    <t xml:space="preserve">Existe una fuerte correlación negativa entre la velocidad del vehículo y su rendimiento</t>
+    <t>Existe una fuerte correlación negativa entre la velocidad del vehículo y su rendimiento</t>
   </si>
   <si>
-    <t xml:space="preserve">¿Por qué fuerte? Porque el valor de r está cerca de -1.</t>
+    <t>¿Por qué fuerte? Porque el valor de r está cerca de -1.</t>
   </si>
   <si>
     <t>Ciudad</t>
   </si>
   <si>
-    <t xml:space="preserve">T max</t>
+    <t>T max</t>
   </si>
   <si>
-    <t xml:space="preserve">T min</t>
+    <t>T min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -83,11 +90,11 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -98,17 +105,20 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -116,11 +126,9 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout/>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -138,27 +146,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+          <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
-            <c:spPr bwMode="auto">
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
+            <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -167,50 +165,28 @@
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="b"/>
-            <c:separator xml:space="preserve"> </c:separator>
-            <c:showBubbleSize val="0"/>
-            <c:showCatName val="1"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="1"/>
-            <c:showVal val="1"/>
-            <c:spPr bwMode="auto">
-              <a:prstGeom prst="rect">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
               </a:ln>
+              <a:effectLst/>
             </c:spPr>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr/>
-              </a:p>
-            </c:txPr>
-          </c:dLbls>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$B$13:$B$22</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>30</c:v>
@@ -242,8 +218,8 @@
                 <c:pt idx="9">
                   <c:v>55</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -285,61 +261,33 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE00-4671-B4F0-E0FF143A5F7D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="b"/>
-          <c:separator xml:space="preserve"> </c:separator>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showCatName val="1"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="1"/>
-          <c:showVal val="1"/>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr/>
-            </a:p>
-          </c:txPr>
         </c:dLbls>
-        <c:axId val="664969007"/>
-        <c:axId val="664969008"/>
+        <c:axId val="297303631"/>
+        <c:axId val="297304047"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="664969007"/>
+        <c:axId val="297303631"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
+          <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -349,16 +297,69 @@
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Velocidad</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
@@ -369,12 +370,14 @@
             </a:solidFill>
             <a:round/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -386,25 +389,22 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664969008"/>
+        <c:crossAx val="297304047"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="664969008"/>
+        <c:axId val="297304047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
-          <c:spPr bwMode="auto">
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
+          <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -414,16 +414,69 @@
               </a:solidFill>
               <a:round/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Rendimiento</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr bwMode="auto">
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
+        <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
@@ -434,12 +487,14 @@
             </a:solidFill>
             <a:round/>
           </a:ln>
+          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -451,67 +506,33 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr/>
+            <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664969007"/>
+        <c:crossAx val="297303631"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr bwMode="auto">
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+      <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="609599" y="4162424"/>
-      <a:ext cx="4552949" cy="2724149"/>
-    </a:xfrm>
-    <a:prstGeom prst="rect">
-      <a:avLst/>
-    </a:prstGeom>
+  <c:spPr>
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
@@ -524,26 +545,21 @@
       </a:solidFill>
       <a:round/>
     </a:ln>
+    <a:effectLst/>
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
+    <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1000">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:latin typeface="+mn-lt"/>
-          <a:ea typeface="+mn-ea"/>
-          <a:cs typeface="+mn-cs"/>
-        </a:defRPr>
+        <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr/>
+      <a:endParaRPr lang="es-MX"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -601,7 +617,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -613,10 +629,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -627,19 +640,16 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="bg1"/>
       </a:solidFill>
@@ -653,7 +663,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -665,8 +675,36 @@
         <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="1">
@@ -696,10 +734,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -719,10 +754,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -730,6 +762,7 @@
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -739,10 +772,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -761,10 +791,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:noFill/>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -776,7 +803,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -785,10 +812,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
           <a:lumMod val="75000"/>
@@ -813,10 +837,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -835,10 +856,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -857,10 +875,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:noFill/>
       <a:ln>
         <a:noFill/>
@@ -874,10 +889,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -896,10 +908,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -918,10 +927,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -940,10 +946,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -965,9 +968,9 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -975,7 +978,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -993,7 +996,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
@@ -1002,10 +1005,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -1027,7 +1027,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" spc="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1038,10 +1038,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1060,7 +1057,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -1069,10 +1066,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
@@ -1097,10 +1091,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
@@ -1111,7 +1102,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -1120,45 +1111,45 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr bwMode="auto">
-      <a:prstGeom prst="rect">
-        <a:avLst/>
-      </a:prstGeom>
+    <cs:spPr>
       <a:noFill/>
       <a:ln>
         <a:noFill/>
       </a:ln>
     </cs:spPr>
   </cs:wall>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
 </cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
-  <xdr:twoCellAnchor editAs="twoCell">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>552449</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="664969002" name="" hidden="0"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{034EA7DC-2C05-20E7-6284-C0650DA24315}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="609599" y="4162424"/>
-        <a:ext cx="4552949" cy="2724149"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1171,291 +1162,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="New Office">
       <a:dk1>
@@ -1658,23 +1366,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A12:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="13.421875"/>
-    <col customWidth="1" min="6" max="6" width="10.00390625"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" ht="14.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -1682,7 +1393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" ht="14.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>30</v>
       </c>
@@ -1692,11 +1403,11 @@
       <c r="E13" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" ht="14.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>50</v>
       </c>
@@ -1707,7 +1418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" ht="14.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>40</v>
       </c>
@@ -1718,7 +1429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" ht="14.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>55</v>
       </c>
@@ -1726,7 +1437,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" ht="14.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>30</v>
       </c>
@@ -1734,7 +1445,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" ht="14.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>25</v>
       </c>
@@ -1742,7 +1453,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" ht="14.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>60</v>
       </c>
@@ -1750,7 +1461,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" ht="14.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>25</v>
       </c>
@@ -1758,7 +1469,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" ht="14.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>50</v>
       </c>
@@ -1766,7 +1477,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" ht="14.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>55</v>
       </c>
@@ -1774,7 +1485,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" ht="14.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1785,81 +1496,79 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" ht="14.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" ht="14.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
     </row>
-    <row r="44" ht="14.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
     </row>
-    <row r="45" ht="14.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>4</v>
       </c>
     </row>
-    <row r="46" ht="14.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5</v>
       </c>
     </row>
-    <row r="47" ht="14.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6</v>
       </c>
     </row>
-    <row r="48" ht="14.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7</v>
       </c>
     </row>
-    <row r="49" ht="14.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>8</v>
       </c>
     </row>
-    <row r="50" ht="14.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>9</v>
       </c>
     </row>
-    <row r="51" ht="14.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>10</v>
       </c>
     </row>
-    <row r="52" ht="14.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>11</v>
       </c>
     </row>
-    <row r="53" ht="14.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>12</v>
       </c>
     </row>
-    <row r="54" ht="14.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>13</v>
       </c>
     </row>
-    <row r="55" ht="14.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" firstPageNumber="4294967295" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>